<commit_message>
Add optimization process, define current performance nad load time,
</commit_message>
<xml_diff>
--- a/tabela-wydajnosci-i-cele.xlsx
+++ b/tabela-wydajnosci-i-cele.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>Ten dokument został wyeksportowany z aplikacji Numbers. Każda z tabel została skonwertowana do arkusza aplikacji Excel. Pozostałe obiekty na każdym z arkuszy Numbers zostały umieszczone na osobnych arkuszach. Pamiętaj, że działanie formuł w aplikacji Excel może być inne.</t>
   </si>
@@ -33,7 +33,32 @@
     <t>Obecny i oczekiwany stan strony WWW</t>
   </si>
   <si>
-    <t xml:space="preserve">Na czym nam zależy_ - Obecny i </t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Na czym nam zależy_ - Obecny i </t>
+    </r>
+  </si>
+  <si>
+    <t>Tabela wydajności</t>
+  </si>
+  <si>
+    <t>Tabela 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Tabela wydajności</t>
+    </r>
   </si>
   <si>
     <t>Czynnik / cecha</t>
@@ -48,28 +73,110 @@
     <t>Nasz cel</t>
   </si>
   <si>
-    <t>Współczynnik odrzuceń strony produktu</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Czas ładowania strony głównej</t>
-  </si>
-  <si>
-    <t>10.5s</t>
-  </si>
-  <si>
-    <t>~5s</t>
-  </si>
-  <si>
-    <t>&lt; 4.5s</t>
-  </si>
-  <si>
-    <t>Tabela wydajności</t>
-  </si>
-  <si>
-    <t>Tabela 1</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Czas ładowania strony głównej </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/</t>
+    </r>
+  </si>
+  <si>
+    <t>25s</t>
+  </si>
+  <si>
+    <t>~10s</t>
+  </si>
+  <si>
+    <t>&lt;7s</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Czas ładowania strony kontaktowej </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/contact.html</t>
+    </r>
+  </si>
+  <si>
+    <t>9.4s</t>
+  </si>
+  <si>
+    <t>~6s</t>
+  </si>
+  <si>
+    <t>&lt;5s</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Czas ładowania strony z newsami </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/news-listing.html</t>
+    </r>
+  </si>
+  <si>
+    <t>~9.3s</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Czas ładowania pojedyńczego newsa </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/news-single.html</t>
+    </r>
+  </si>
+  <si>
+    <t>11.5s</t>
+  </si>
+  <si>
+    <t>3.5s</t>
+  </si>
+  <si>
+    <t>~3s</t>
   </si>
   <si>
     <t>TTFB</t>
@@ -96,16 +203,124 @@
     <t>Lighthouse</t>
   </si>
   <si>
-    <t>Typ strony 1</t>
-  </si>
-  <si>
-    <t>Typ strony 2</t>
-  </si>
-  <si>
-    <t>Typ strony 3</t>
-  </si>
-  <si>
-    <t>Typ strony 4</t>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Strona główna </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="20"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">14,965
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Kontakt </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/contact.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="20"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">6,299
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="20"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">0.457
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">News </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/news-listing.html</t>
+    </r>
+  </si>
+  <si>
+    <t>0.378</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Pojedynczy news </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/news-single.html</t>
+    </r>
   </si>
   <si>
     <t>Zmienność</t>
@@ -115,10 +330,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="[s]&quot;s&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -130,6 +346,11 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -137,7 +358,7 @@
     <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="11"/>
+      <color indexed="12"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -147,14 +368,10 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <u val="single"/>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
+      <color indexed="12"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
       <b val="1"/>
@@ -162,19 +379,30 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b val="1"/>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="20"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -184,7 +412,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="11"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -196,13 +430,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="16"/>
+        <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="21"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -218,30 +470,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="19"/>
+        <fgColor indexed="23"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="20"/>
+        <fgColor indexed="24"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="21"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="22"/>
+        <fgColor indexed="25"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -251,116 +497,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="14"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -369,7 +510,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -377,19 +518,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </top>
-      <bottom style="thin">
-        <color indexed="17"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </left>
       <right/>
       <top/>
@@ -404,30 +543,236 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -437,107 +782,212 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="12" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -557,23 +1007,74 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="015e88b1"/>
-      <rgbColor rgb="01eef3f4"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffd5d5d5"/>
-      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="fff9f9f9"/>
-      <rgbColor rgb="fffe634d"/>
-      <rgbColor rgb="ff88f94e"/>
-      <rgbColor rgb="ffff968c"/>
+      <rgbColor rgb="ff222222"/>
+      <rgbColor rgb="ffff644e"/>
+      <rgbColor rgb="ff16e7cf"/>
+      <rgbColor rgb="ffffb1a6"/>
+      <rgbColor rgb="ffff8a7a"/>
       <rgbColor rgb="ffed220b"/>
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>384340</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>158165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>824699</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66624</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Shape 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4397540" y="3258235"/>
+          <a:ext cx="440360" cy="250090"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,10 +1088,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -767,11 +1268,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -780,34 +1284,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1055,12 +1559,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1351,7 +1855,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1629,73 +2133,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="4" width="33.6719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="14.7" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" ht="14.7" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+    </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="5"/>
+      <c r="B3" t="s" s="8">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" ht="18.6" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" t="s" s="9">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="9">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" ht="16.65" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s" s="10">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" ht="30.65" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="12"/>
+      <c r="C10" t="s" s="13">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="D10" t="s" s="14">
         <v>6</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
-      <c r="C12" t="s" s="4">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s" s="5">
-        <v>17</v>
-      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" ht="16.65" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s" s="10">
+        <v>7</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" ht="16.65" customHeight="1">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" t="s" s="17">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s" s="18">
+        <v>9</v>
+      </c>
+      <c r="E12" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'Na czym nam zależy_ - Obecny i '!R2C1" tooltip="" display="Na czym nam zależy_ - Obecny i "/>
+    <hyperlink ref="D10" location="'Na czym nam zależy_ - Obecny i '!R1C1" tooltip="" display="Na czym nam zależy_ - Obecny i "/>
     <hyperlink ref="D12" location="'Tabela wydajności'!R1C1" tooltip="" display="Tabela wydajności"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1704,117 +2273,149 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="55.9219" style="6" customWidth="1"/>
-    <col min="2" max="2" width="31.4062" style="6" customWidth="1"/>
-    <col min="3" max="3" width="32.2031" style="6" customWidth="1"/>
-    <col min="4" max="4" width="29.8438" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="16.3516" style="6" customWidth="1"/>
+    <col min="1" max="1" width="56" style="20" customWidth="1"/>
+    <col min="2" max="2" width="31.5" style="20" customWidth="1"/>
+    <col min="3" max="3" width="32.1719" style="20" customWidth="1"/>
+    <col min="4" max="4" width="29.8516" style="20" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="7">
+      <c r="A1" t="s" s="21">
         <v>5</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="8">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s" s="8">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s" s="8">
+      <c r="A2" t="s" s="24">
         <v>10</v>
       </c>
+      <c r="B2" t="s" s="24">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s" s="24">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s" s="24">
+        <v>13</v>
+      </c>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="B3" s="10">
-        <v>0.92</v>
-      </c>
-      <c r="C3" t="s" s="11">
-        <v>12</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0.75</v>
-      </c>
+      <c r="A3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="13">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s" s="14">
+      <c r="A4" t="s" s="30">
         <v>14</v>
       </c>
-      <c r="C4" t="s" s="15">
+      <c r="B4" t="s" s="31">
         <v>15</v>
       </c>
-      <c r="D4" t="s" s="15">
+      <c r="C4" t="s" s="32">
         <v>16</v>
       </c>
+      <c r="D4" t="s" s="32">
+        <v>17</v>
+      </c>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="A5" t="s" s="30">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s" s="31">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s" s="32">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="A6" t="s" s="30">
+        <v>22</v>
+      </c>
+      <c r="B6" s="33">
+        <v>0.0002314814814814815</v>
+      </c>
+      <c r="C6" t="s" s="32">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s" s="32">
+        <v>17</v>
+      </c>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
+      <c r="A7" t="s" s="30">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s" s="34">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="32">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="32">
+        <v>27</v>
+      </c>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="25"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="25"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/"/>
+    <hyperlink ref="A5" r:id="rId2" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/contact.html"/>
+    <hyperlink ref="A6" r:id="rId3" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/news-listing.html"/>
+    <hyperlink ref="A7" r:id="rId4" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/news-single.html"/>
+  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -1831,243 +2432,250 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.3984" style="19" customWidth="1"/>
-    <col min="2" max="2" width="17.9141" style="19" customWidth="1"/>
-    <col min="3" max="3" width="15.3516" style="19" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="19" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="19" customWidth="1"/>
-    <col min="6" max="6" width="15.3516" style="19" customWidth="1"/>
-    <col min="7" max="8" width="16.3516" style="19" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="14.5" style="19" customWidth="1"/>
+    <col min="1" max="1" width="19.3516" style="39" customWidth="1"/>
+    <col min="2" max="2" width="18" style="39" customWidth="1"/>
+    <col min="3" max="3" width="15.3516" style="39" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="39" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="39" customWidth="1"/>
+    <col min="6" max="6" width="15.3516" style="39" customWidth="1"/>
+    <col min="7" max="8" width="16.3516" style="39" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="39" customWidth="1"/>
+    <col min="10" max="16384" width="14.5" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="20"/>
-      <c r="B1" t="s" s="21">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s" s="21">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s" s="21">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s" s="21">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s" s="21">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s" s="21">
-        <v>24</v>
-      </c>
-      <c r="H1" t="s" s="21">
-        <v>25</v>
-      </c>
-      <c r="I1" t="s" s="22">
-        <v>26</v>
+      <c r="A1" s="40"/>
+      <c r="B1" t="s" s="41">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s" s="41">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s" s="41">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s" s="41">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s" s="41">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s" s="41">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s" s="41">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s" s="42">
+        <v>35</v>
       </c>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="23">
-        <v>27</v>
-      </c>
-      <c r="B2" s="24">
-        <v>1.164</v>
-      </c>
-      <c r="C2" s="24">
-        <v>1.8</v>
-      </c>
-      <c r="D2" s="24">
-        <v>3.139</v>
-      </c>
-      <c r="E2" s="24">
-        <v>4.791</v>
-      </c>
-      <c r="F2" s="24">
-        <v>1.073</v>
-      </c>
-      <c r="G2" s="24">
-        <v>0.032</v>
-      </c>
-      <c r="H2" s="24">
+      <c r="A2" t="s" s="43">
+        <v>36</v>
+      </c>
+      <c r="B2" s="44">
+        <v>0.169</v>
+      </c>
+      <c r="C2" s="44">
+        <v>1.1</v>
+      </c>
+      <c r="D2" s="44">
+        <v>1.048</v>
+      </c>
+      <c r="E2" s="45">
+        <v>11.607</v>
+      </c>
+      <c r="F2" t="s" s="47">
+        <v>37</v>
+      </c>
+      <c r="G2" s="48">
+        <v>0.091</v>
+      </c>
+      <c r="H2" s="49">
         <v>0.106</v>
       </c>
-      <c r="I2" s="25">
-        <v>15</v>
+      <c r="I2" s="50">
+        <v>9</v>
       </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="23">
-        <v>28</v>
-      </c>
-      <c r="B3" s="24">
-        <v>1.78</v>
-      </c>
-      <c r="C3" s="26">
-        <v>6.281</v>
-      </c>
-      <c r="D3" s="24">
-        <v>3.901</v>
-      </c>
-      <c r="E3" s="26">
-        <v>6.781</v>
-      </c>
-      <c r="F3" s="26">
-        <v>18.98</v>
-      </c>
-      <c r="G3" s="27">
-        <v>1.036</v>
-      </c>
-      <c r="H3" s="24">
-        <v>0.128</v>
-      </c>
-      <c r="I3" s="25">
+      <c r="A3" t="s" s="43">
+        <v>38</v>
+      </c>
+      <c r="B3" s="44">
+        <v>0.242</v>
+      </c>
+      <c r="C3" s="51">
+        <v>1.1</v>
+      </c>
+      <c r="D3" s="44">
+        <v>1.037</v>
+      </c>
+      <c r="E3" s="52">
+        <v>5.98</v>
+      </c>
+      <c r="F3" t="s" s="54">
+        <v>39</v>
+      </c>
+      <c r="G3" s="55">
+        <v>0.005</v>
+      </c>
+      <c r="H3" t="s" s="57">
+        <v>40</v>
+      </c>
+      <c r="I3" s="50">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" t="s" s="43">
+        <v>41</v>
+      </c>
+      <c r="B4" s="44">
+        <v>0.248</v>
+      </c>
+      <c r="C4" s="44">
+        <v>1.1</v>
+      </c>
+      <c r="D4" s="44">
+        <v>1.089</v>
+      </c>
+      <c r="E4" s="44">
+        <v>11.2</v>
+      </c>
+      <c r="F4" s="58">
+        <v>10.667</v>
+      </c>
+      <c r="G4" s="59">
+        <v>0.194</v>
+      </c>
+      <c r="H4" t="s" s="60">
+        <v>42</v>
+      </c>
+      <c r="I4" s="50">
         <v>6</v>
       </c>
     </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="23">
-        <v>29</v>
-      </c>
-      <c r="B4" s="24">
-        <v>1.261</v>
-      </c>
-      <c r="C4" s="24">
-        <v>1.9</v>
-      </c>
-      <c r="D4" s="24">
-        <v>3.91</v>
-      </c>
-      <c r="E4" s="24">
-        <v>4.776</v>
-      </c>
-      <c r="F4" s="24">
-        <v>3.215</v>
-      </c>
-      <c r="G4" s="24">
-        <v>0.005</v>
-      </c>
-      <c r="H4" s="24">
-        <v>0.663</v>
-      </c>
-      <c r="I4" s="25">
-        <v>34</v>
-      </c>
-    </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="23">
-        <v>30</v>
-      </c>
-      <c r="B5" s="24">
-        <v>1.787</v>
-      </c>
-      <c r="C5" s="24">
-        <v>3.148</v>
-      </c>
-      <c r="D5" s="24">
-        <v>3.21</v>
-      </c>
-      <c r="E5" s="24">
-        <v>5.021</v>
-      </c>
-      <c r="F5" s="24">
-        <v>2.648</v>
-      </c>
-      <c r="G5" s="24">
-        <v>0.876</v>
-      </c>
-      <c r="H5" s="24">
-        <v>0.125</v>
-      </c>
-      <c r="I5" s="25">
+      <c r="A5" t="s" s="43">
+        <v>43</v>
+      </c>
+      <c r="B5" s="49">
+        <v>0.329</v>
+      </c>
+      <c r="C5" s="49">
+        <v>1.1</v>
+      </c>
+      <c r="D5" s="49">
+        <v>1.134</v>
+      </c>
+      <c r="E5" s="49">
+        <v>5.902</v>
+      </c>
+      <c r="F5" s="61">
+        <v>7.458</v>
+      </c>
+      <c r="G5" s="59">
+        <v>0.201</v>
+      </c>
+      <c r="H5" s="62">
+        <v>0.376</v>
+      </c>
+      <c r="I5" s="50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" t="s" s="43">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="23">
-        <v>31</v>
-      </c>
-      <c r="B6" s="28">
+      <c r="B6" s="63">
         <f>STDEV(B2:B5)</f>
-        <v>0.332049193142623</v>
-      </c>
-      <c r="C6" s="27">
+        <v>0.0654064217030713</v>
+      </c>
+      <c r="C6" s="63">
         <f>STDEV(C2:C5)</f>
-        <v>2.09110853775376</v>
-      </c>
-      <c r="D6" s="24">
+        <v>0</v>
+      </c>
+      <c r="D6" s="63">
         <f>STDEV(D2:D5)</f>
-        <v>0.423053188145415</v>
-      </c>
-      <c r="E6" s="29">
+        <v>0.0440983748755741</v>
+      </c>
+      <c r="E6" s="64">
         <f>STDEV(E2:E5)</f>
-        <v>0.96569814987224</v>
-      </c>
-      <c r="F6" s="30">
+        <v>3.15831034732181</v>
+      </c>
+      <c r="F6" s="65">
         <f>STDEV(F2:F5)</f>
-        <v>8.38311982498163</v>
-      </c>
-      <c r="G6" s="24">
+        <v>2.26910566082763</v>
+      </c>
+      <c r="G6" s="62">
         <f>STDEV(G2:G5)</f>
-        <v>0.545304425680433</v>
-      </c>
-      <c r="H6" s="28">
+        <v>0.0932250860373251</v>
+      </c>
+      <c r="H6" s="62">
         <f>STDEV(H2:H5)</f>
-        <v>0.271841252694779</v>
-      </c>
-      <c r="I6" s="31"/>
+        <v>0.190918830920368</v>
+      </c>
+      <c r="I6" s="66"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="68"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
+      <c r="A9" s="68"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
+      <c r="A10" s="68"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/"/>
+    <hyperlink ref="A3" r:id="rId2" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/contact.html"/>
+    <hyperlink ref="A4" r:id="rId3" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/news-listing.html"/>
+    <hyperlink ref="A5" r:id="rId4" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/news-single.html"/>
+  </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Move scripts at bottom with defer
</commit_message>
<xml_diff>
--- a/tabela-wydajnosci-i-cele.xlsx
+++ b/tabela-wydajnosci-i-cele.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
   <si>
     <t>Ten dokument został wyeksportowany z aplikacji Numbers. Każda z tabel została skonwertowana do arkusza aplikacji Excel. Pozostałe obiekty na każdym z arkuszy Numbers zostały umieszczone na osobnych arkuszach. Pamiętaj, że działanie formuł w aplikacji Excel może być inne.</t>
   </si>
@@ -33,7 +33,32 @@
     <t>Obecny i oczekiwany stan strony WWW</t>
   </si>
   <si>
-    <t xml:space="preserve">Na czym nam zależy_ - Obecny i </t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Na czym nam zależy_ - Obecny i </t>
+    </r>
+  </si>
+  <si>
+    <t>Tabela wydajności</t>
+  </si>
+  <si>
+    <t>Tabela 1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Tabela wydajności</t>
+    </r>
   </si>
   <si>
     <t>Czynnik / cecha</t>
@@ -48,28 +73,110 @@
     <t>Nasz cel</t>
   </si>
   <si>
-    <t>Współczynnik odrzuceń strony produktu</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Czas ładowania strony głównej</t>
-  </si>
-  <si>
-    <t>10.5s</t>
-  </si>
-  <si>
-    <t>~5s</t>
-  </si>
-  <si>
-    <t>&lt; 4.5s</t>
-  </si>
-  <si>
-    <t>Tabela wydajności</t>
-  </si>
-  <si>
-    <t>Tabela 1</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Czas ładowania strony głównej </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/</t>
+    </r>
+  </si>
+  <si>
+    <t>25s</t>
+  </si>
+  <si>
+    <t>~10s</t>
+  </si>
+  <si>
+    <t>&lt;7s</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Czas ładowania strony kontaktowej </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/contact.html</t>
+    </r>
+  </si>
+  <si>
+    <t>9.4s</t>
+  </si>
+  <si>
+    <t>~6s</t>
+  </si>
+  <si>
+    <t>&lt;5s</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Czas ładowania strony z newsami </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/news-listing.html</t>
+    </r>
+  </si>
+  <si>
+    <t>~9.3s</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Czas ładowania pojedyńczego newsa </t>
+    </r>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/news-single.html</t>
+    </r>
+  </si>
+  <si>
+    <t>11.5s</t>
+  </si>
+  <si>
+    <t>3.5s</t>
+  </si>
+  <si>
+    <t>~3s</t>
   </si>
   <si>
     <t>TTFB</t>
@@ -96,16 +203,124 @@
     <t>Lighthouse</t>
   </si>
   <si>
-    <t>Typ strony 1</t>
-  </si>
-  <si>
-    <t>Typ strony 2</t>
-  </si>
-  <si>
-    <t>Typ strony 3</t>
-  </si>
-  <si>
-    <t>Typ strony 4</t>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Strona główna </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="20"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">14,965
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Kontakt </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/contact.html</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="20"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">6,299
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="20"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">0.457
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">News </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/news-listing.html</t>
+    </r>
+  </si>
+  <si>
+    <t>0.378</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">Pojedynczy news </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="1"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>https://wdi-optimised-frontend-starter.vercel.app/news-single.html</t>
+    </r>
   </si>
   <si>
     <t>Zmienność</t>
@@ -115,10 +330,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="0" formatCode="General"/>
+    <numFmt numFmtId="59" formatCode="[s]&quot;s&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -130,6 +346,11 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -137,7 +358,7 @@
     <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="11"/>
+      <color indexed="12"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -147,14 +368,10 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <u val="single"/>
       <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
+      <color indexed="12"/>
+      <name val="Helvetica Neue"/>
     </font>
     <font>
       <b val="1"/>
@@ -162,19 +379,30 @@
       <color indexed="8"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <b val="1"/>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="20"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -184,7 +412,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="12"/>
+        <fgColor indexed="11"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="13"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -196,13 +430,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="16"/>
+        <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="18"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="19"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="21"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="22"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -218,30 +470,24 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="19"/>
+        <fgColor indexed="23"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="20"/>
+        <fgColor indexed="24"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="21"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="22"/>
+        <fgColor indexed="25"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -251,116 +497,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="14"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="14"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="14"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="14"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="13"/>
-      </left>
-      <right style="thin">
-        <color indexed="13"/>
-      </right>
-      <top style="thin">
-        <color indexed="13"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="13"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -369,7 +510,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -377,19 +518,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </top>
-      <bottom style="thin">
-        <color indexed="17"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </left>
       <right/>
       <top/>
@@ -404,30 +543,236 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="17"/>
+        <color indexed="9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="17"/>
+        <color indexed="14"/>
       </right>
       <top style="thin">
-        <color indexed="17"/>
+        <color indexed="14"/>
       </top>
       <bottom style="thin">
-        <color indexed="17"/>
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="14"/>
+      </right>
+      <top style="thin">
+        <color indexed="14"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="14"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="14"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="9"/>
+      </right>
+      <top style="thin">
+        <color indexed="9"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="9"/>
       </bottom>
       <diagonal/>
     </border>
@@ -437,107 +782,212 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="12" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="12" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="5" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -557,23 +1007,74 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="015e88b1"/>
-      <rgbColor rgb="01eef3f4"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
       <rgbColor rgb="ffd5d5d5"/>
-      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="fff9f9f9"/>
-      <rgbColor rgb="fffe634d"/>
-      <rgbColor rgb="ff88f94e"/>
-      <rgbColor rgb="ffff968c"/>
+      <rgbColor rgb="ff222222"/>
+      <rgbColor rgb="ffff644e"/>
+      <rgbColor rgb="ff16e7cf"/>
+      <rgbColor rgb="ffffb1a6"/>
+      <rgbColor rgb="ffff8a7a"/>
       <rgbColor rgb="ffed220b"/>
     </indexedColors>
   </colors>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>384340</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>158165</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>824699</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>66624</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp>
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Shape 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4397540" y="3258235"/>
+          <a:ext cx="440360" cy="250090"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -587,10 +1088,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -767,11 +1268,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -780,34 +1284,34 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1055,12 +1559,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1351,7 +1855,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1629,73 +2133,138 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="2" customWidth="1"/>
-    <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="1" max="1" width="2" style="1" customWidth="1"/>
+    <col min="2" max="4" width="33.6719" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="14.7" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
+    </row>
+    <row r="2" ht="14.7" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7"/>
+    </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="5"/>
+      <c r="B3" t="s" s="8">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-    </row>
-    <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="7"/>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" s="5"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="5"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" ht="18.6" customHeight="1">
+      <c r="A7" s="5"/>
+      <c r="B7" t="s" s="9">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="9">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="9">
         <v>3</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" t="s" s="3">
+      <c r="E7" s="7"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7"/>
+    </row>
+    <row r="9" ht="16.65" customHeight="1">
+      <c r="A9" s="5"/>
+      <c r="B9" t="s" s="10">
         <v>4</v>
       </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="7"/>
+    </row>
+    <row r="10" ht="30.65" customHeight="1">
+      <c r="A10" s="5"/>
+      <c r="B10" s="12"/>
+      <c r="C10" t="s" s="13">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
+      <c r="D10" t="s" s="14">
         <v>6</v>
       </c>
-    </row>
-    <row r="11">
-      <c r="B11" t="s" s="3">
-        <v>17</v>
-      </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12">
-      <c r="B12" s="4"/>
-      <c r="C12" t="s" s="4">
-        <v>18</v>
-      </c>
-      <c r="D12" t="s" s="5">
-        <v>17</v>
-      </c>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" ht="16.65" customHeight="1">
+      <c r="A11" s="5"/>
+      <c r="B11" t="s" s="10">
+        <v>7</v>
+      </c>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" ht="16.65" customHeight="1">
+      <c r="A12" s="15"/>
+      <c r="B12" s="16"/>
+      <c r="C12" t="s" s="17">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s" s="18">
+        <v>9</v>
+      </c>
+      <c r="E12" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'Na czym nam zależy_ - Obecny i '!R2C1" tooltip="" display="Na czym nam zależy_ - Obecny i "/>
+    <hyperlink ref="D10" location="'Na czym nam zależy_ - Obecny i '!R1C1" tooltip="" display="Na czym nam zależy_ - Obecny i "/>
     <hyperlink ref="D12" location="'Tabela wydajności'!R1C1" tooltip="" display="Tabela wydajności"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1704,117 +2273,149 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="55.9219" style="6" customWidth="1"/>
-    <col min="2" max="2" width="31.4062" style="6" customWidth="1"/>
-    <col min="3" max="3" width="32.2031" style="6" customWidth="1"/>
-    <col min="4" max="4" width="29.8438" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="16.3516" style="6" customWidth="1"/>
+    <col min="1" max="1" width="56" style="20" customWidth="1"/>
+    <col min="2" max="2" width="31.5" style="20" customWidth="1"/>
+    <col min="3" max="3" width="32.1719" style="20" customWidth="1"/>
+    <col min="4" max="4" width="29.8516" style="20" customWidth="1"/>
+    <col min="5" max="5" width="16.3516" style="20" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="7">
+      <c r="A1" t="s" s="21">
         <v>5</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="8">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s" s="8">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s" s="8">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s" s="8">
+      <c r="A2" t="s" s="24">
         <v>10</v>
       </c>
+      <c r="B2" t="s" s="24">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s" s="24">
+        <v>12</v>
+      </c>
+      <c r="D2" t="s" s="24">
+        <v>13</v>
+      </c>
+      <c r="E2" s="25"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" t="s" s="9">
-        <v>11</v>
-      </c>
-      <c r="B3" s="10">
-        <v>0.92</v>
-      </c>
-      <c r="C3" t="s" s="11">
-        <v>12</v>
-      </c>
-      <c r="D3" s="12">
-        <v>0.75</v>
-      </c>
+      <c r="A3" s="26"/>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="25"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="13">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s" s="14">
+      <c r="A4" t="s" s="30">
         <v>14</v>
       </c>
-      <c r="C4" t="s" s="15">
+      <c r="B4" t="s" s="31">
         <v>15</v>
       </c>
-      <c r="D4" t="s" s="15">
+      <c r="C4" t="s" s="32">
         <v>16</v>
       </c>
+      <c r="D4" t="s" s="32">
+        <v>17</v>
+      </c>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
+      <c r="A5" t="s" s="30">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s" s="31">
+        <v>19</v>
+      </c>
+      <c r="C5" t="s" s="32">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="E5" s="25"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="16"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
+      <c r="A6" t="s" s="30">
+        <v>22</v>
+      </c>
+      <c r="B6" s="33">
+        <v>0.0002314814814814815</v>
+      </c>
+      <c r="C6" t="s" s="32">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s" s="32">
+        <v>17</v>
+      </c>
+      <c r="E6" s="25"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="16"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
+      <c r="A7" t="s" s="30">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s" s="34">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="32">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s" s="32">
+        <v>27</v>
+      </c>
+      <c r="E7" s="25"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="16"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="25"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="37"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="25"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="25"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="16"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="18"/>
-      <c r="D11" s="18"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A4" r:id="rId1" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/"/>
+    <hyperlink ref="A5" r:id="rId2" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/contact.html"/>
+    <hyperlink ref="A6" r:id="rId3" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/news-listing.html"/>
+    <hyperlink ref="A7" r:id="rId4" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/news-single.html"/>
+  </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
@@ -1831,243 +2432,250 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.3984" style="19" customWidth="1"/>
-    <col min="2" max="2" width="17.9141" style="19" customWidth="1"/>
-    <col min="3" max="3" width="15.3516" style="19" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="19" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="19" customWidth="1"/>
-    <col min="6" max="6" width="15.3516" style="19" customWidth="1"/>
-    <col min="7" max="8" width="16.3516" style="19" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="19" customWidth="1"/>
-    <col min="10" max="16384" width="14.5" style="19" customWidth="1"/>
+    <col min="1" max="1" width="19.3516" style="39" customWidth="1"/>
+    <col min="2" max="2" width="18" style="39" customWidth="1"/>
+    <col min="3" max="3" width="15.3516" style="39" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="39" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="39" customWidth="1"/>
+    <col min="6" max="6" width="15.3516" style="39" customWidth="1"/>
+    <col min="7" max="8" width="16.3516" style="39" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="39" customWidth="1"/>
+    <col min="10" max="16384" width="14.5" style="39" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="20"/>
-      <c r="B1" t="s" s="21">
-        <v>19</v>
-      </c>
-      <c r="C1" t="s" s="21">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s" s="21">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s" s="21">
-        <v>22</v>
-      </c>
-      <c r="F1" t="s" s="21">
-        <v>23</v>
-      </c>
-      <c r="G1" t="s" s="21">
-        <v>24</v>
-      </c>
-      <c r="H1" t="s" s="21">
-        <v>25</v>
-      </c>
-      <c r="I1" t="s" s="22">
-        <v>26</v>
+      <c r="A1" s="40"/>
+      <c r="B1" t="s" s="41">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s" s="41">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s" s="41">
+        <v>30</v>
+      </c>
+      <c r="E1" t="s" s="41">
+        <v>31</v>
+      </c>
+      <c r="F1" t="s" s="41">
+        <v>32</v>
+      </c>
+      <c r="G1" t="s" s="41">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s" s="41">
+        <v>34</v>
+      </c>
+      <c r="I1" t="s" s="42">
+        <v>35</v>
       </c>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="23">
-        <v>27</v>
-      </c>
-      <c r="B2" s="24">
-        <v>1.164</v>
-      </c>
-      <c r="C2" s="24">
-        <v>1.8</v>
-      </c>
-      <c r="D2" s="24">
-        <v>3.139</v>
-      </c>
-      <c r="E2" s="24">
-        <v>4.791</v>
-      </c>
-      <c r="F2" s="24">
-        <v>1.073</v>
-      </c>
-      <c r="G2" s="24">
-        <v>0.032</v>
-      </c>
-      <c r="H2" s="24">
+      <c r="A2" t="s" s="43">
+        <v>36</v>
+      </c>
+      <c r="B2" s="44">
+        <v>0.169</v>
+      </c>
+      <c r="C2" s="44">
+        <v>1.1</v>
+      </c>
+      <c r="D2" s="44">
+        <v>1.048</v>
+      </c>
+      <c r="E2" s="45">
+        <v>11.607</v>
+      </c>
+      <c r="F2" t="s" s="47">
+        <v>37</v>
+      </c>
+      <c r="G2" s="48">
+        <v>0.091</v>
+      </c>
+      <c r="H2" s="49">
         <v>0.106</v>
       </c>
-      <c r="I2" s="25">
-        <v>15</v>
+      <c r="I2" s="50">
+        <v>9</v>
       </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="23">
-        <v>28</v>
-      </c>
-      <c r="B3" s="24">
-        <v>1.78</v>
-      </c>
-      <c r="C3" s="26">
-        <v>6.281</v>
-      </c>
-      <c r="D3" s="24">
-        <v>3.901</v>
-      </c>
-      <c r="E3" s="26">
-        <v>6.781</v>
-      </c>
-      <c r="F3" s="26">
-        <v>18.98</v>
-      </c>
-      <c r="G3" s="27">
-        <v>1.036</v>
-      </c>
-      <c r="H3" s="24">
-        <v>0.128</v>
-      </c>
-      <c r="I3" s="25">
+      <c r="A3" t="s" s="43">
+        <v>38</v>
+      </c>
+      <c r="B3" s="44">
+        <v>0.242</v>
+      </c>
+      <c r="C3" s="51">
+        <v>1.1</v>
+      </c>
+      <c r="D3" s="44">
+        <v>1.037</v>
+      </c>
+      <c r="E3" s="52">
+        <v>5.98</v>
+      </c>
+      <c r="F3" t="s" s="54">
+        <v>39</v>
+      </c>
+      <c r="G3" s="55">
+        <v>0.005</v>
+      </c>
+      <c r="H3" t="s" s="57">
+        <v>40</v>
+      </c>
+      <c r="I3" s="50">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" ht="13.65" customHeight="1">
+      <c r="A4" t="s" s="43">
+        <v>41</v>
+      </c>
+      <c r="B4" s="44">
+        <v>0.248</v>
+      </c>
+      <c r="C4" s="44">
+        <v>1.1</v>
+      </c>
+      <c r="D4" s="44">
+        <v>1.089</v>
+      </c>
+      <c r="E4" s="44">
+        <v>11.2</v>
+      </c>
+      <c r="F4" s="58">
+        <v>10.667</v>
+      </c>
+      <c r="G4" s="59">
+        <v>0.194</v>
+      </c>
+      <c r="H4" t="s" s="60">
+        <v>42</v>
+      </c>
+      <c r="I4" s="50">
         <v>6</v>
       </c>
     </row>
-    <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="23">
-        <v>29</v>
-      </c>
-      <c r="B4" s="24">
-        <v>1.261</v>
-      </c>
-      <c r="C4" s="24">
-        <v>1.9</v>
-      </c>
-      <c r="D4" s="24">
-        <v>3.91</v>
-      </c>
-      <c r="E4" s="24">
-        <v>4.776</v>
-      </c>
-      <c r="F4" s="24">
-        <v>3.215</v>
-      </c>
-      <c r="G4" s="24">
-        <v>0.005</v>
-      </c>
-      <c r="H4" s="24">
-        <v>0.663</v>
-      </c>
-      <c r="I4" s="25">
-        <v>34</v>
-      </c>
-    </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="23">
-        <v>30</v>
-      </c>
-      <c r="B5" s="24">
-        <v>1.787</v>
-      </c>
-      <c r="C5" s="24">
-        <v>3.148</v>
-      </c>
-      <c r="D5" s="24">
-        <v>3.21</v>
-      </c>
-      <c r="E5" s="24">
-        <v>5.021</v>
-      </c>
-      <c r="F5" s="24">
-        <v>2.648</v>
-      </c>
-      <c r="G5" s="24">
-        <v>0.876</v>
-      </c>
-      <c r="H5" s="24">
-        <v>0.125</v>
-      </c>
-      <c r="I5" s="25">
+      <c r="A5" t="s" s="43">
+        <v>43</v>
+      </c>
+      <c r="B5" s="49">
+        <v>0.329</v>
+      </c>
+      <c r="C5" s="49">
+        <v>1.1</v>
+      </c>
+      <c r="D5" s="49">
+        <v>1.134</v>
+      </c>
+      <c r="E5" s="49">
+        <v>5.902</v>
+      </c>
+      <c r="F5" s="61">
+        <v>7.458</v>
+      </c>
+      <c r="G5" s="59">
+        <v>0.201</v>
+      </c>
+      <c r="H5" s="62">
+        <v>0.376</v>
+      </c>
+      <c r="I5" s="50">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" ht="13.65" customHeight="1">
+      <c r="A6" t="s" s="43">
         <v>44</v>
       </c>
-    </row>
-    <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="23">
-        <v>31</v>
-      </c>
-      <c r="B6" s="28">
+      <c r="B6" s="63">
         <f>STDEV(B2:B5)</f>
-        <v>0.332049193142623</v>
-      </c>
-      <c r="C6" s="27">
+        <v>0.0654064217030713</v>
+      </c>
+      <c r="C6" s="63">
         <f>STDEV(C2:C5)</f>
-        <v>2.09110853775376</v>
-      </c>
-      <c r="D6" s="24">
+        <v>0</v>
+      </c>
+      <c r="D6" s="63">
         <f>STDEV(D2:D5)</f>
-        <v>0.423053188145415</v>
-      </c>
-      <c r="E6" s="29">
+        <v>0.0440983748755741</v>
+      </c>
+      <c r="E6" s="64">
         <f>STDEV(E2:E5)</f>
-        <v>0.96569814987224</v>
-      </c>
-      <c r="F6" s="30">
+        <v>3.15831034732181</v>
+      </c>
+      <c r="F6" s="65">
         <f>STDEV(F2:F5)</f>
-        <v>8.38311982498163</v>
-      </c>
-      <c r="G6" s="24">
+        <v>2.26910566082763</v>
+      </c>
+      <c r="G6" s="62">
         <f>STDEV(G2:G5)</f>
-        <v>0.545304425680433</v>
-      </c>
-      <c r="H6" s="28">
+        <v>0.0932250860373251</v>
+      </c>
+      <c r="H6" s="62">
         <f>STDEV(H2:H5)</f>
-        <v>0.271841252694779</v>
-      </c>
-      <c r="I6" s="31"/>
+        <v>0.190918830920368</v>
+      </c>
+      <c r="I6" s="66"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="33"/>
+      <c r="A7" s="67"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="68"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="33"/>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="33"/>
-      <c r="I8" s="33"/>
+      <c r="A8" s="68"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="33"/>
-      <c r="B9" s="33"/>
-      <c r="C9" s="33"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="33"/>
-      <c r="G9" s="33"/>
-      <c r="H9" s="33"/>
-      <c r="I9" s="33"/>
+      <c r="A9" s="68"/>
+      <c r="B9" s="68"/>
+      <c r="C9" s="68"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="33"/>
-      <c r="B10" s="33"/>
-      <c r="C10" s="33"/>
-      <c r="D10" s="33"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="33"/>
-      <c r="G10" s="33"/>
-      <c r="H10" s="33"/>
-      <c r="I10" s="33"/>
+      <c r="A10" s="68"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/"/>
+    <hyperlink ref="A3" r:id="rId2" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/contact.html"/>
+    <hyperlink ref="A4" r:id="rId3" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/news-listing.html"/>
+    <hyperlink ref="A5" r:id="rId4" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/news-single.html"/>
+  </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update speed test result after optimize script loading
</commit_message>
<xml_diff>
--- a/tabela-wydajnosci-i-cele.xlsx
+++ b/tabela-wydajnosci-i-cele.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="49">
   <si>
     <t>Ten dokument został wyeksportowany z aplikacji Numbers. Każda z tabel została skonwertowana do arkusza aplikacji Excel. Pozostałe obiekty na każdym z arkuszy Numbers zostały umieszczone na osobnych arkuszach. Pamiętaj, że działanie formuł w aplikacji Excel może być inne.</t>
   </si>
@@ -37,7 +37,7 @@
       <rPr>
         <u val="single"/>
         <sz val="12"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t xml:space="preserve">Na czym nam zależy_ - Obecny i </t>
@@ -54,7 +54,7 @@
       <rPr>
         <u val="single"/>
         <sz val="12"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>Tabela wydajności</t>
@@ -85,7 +85,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://wdi-optimised-frontend-starter.vercel.app/</t>
@@ -113,7 +113,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://wdi-optimised-frontend-starter.vercel.app/contact.html</t>
@@ -141,7 +141,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://wdi-optimised-frontend-starter.vercel.app/news-listing.html</t>
@@ -163,7 +163,7 @@
       <rPr>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Helvetica Neue"/>
       </rPr>
       <t>https://wdi-optimised-frontend-starter.vercel.app/news-single.html</t>
@@ -217,7 +217,7 @@
         <b val="1"/>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Arial"/>
       </rPr>
       <t>https://wdi-optimised-frontend-starter.vercel.app/</t>
@@ -249,7 +249,7 @@
         <b val="1"/>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Arial"/>
       </rPr>
       <t>https://wdi-optimised-frontend-starter.vercel.app/contact.html</t>
@@ -292,7 +292,7 @@
         <b val="1"/>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Arial"/>
       </rPr>
       <t>https://wdi-optimised-frontend-starter.vercel.app/news-listing.html</t>
@@ -316,7 +316,7 @@
         <b val="1"/>
         <u val="single"/>
         <sz val="10"/>
-        <color indexed="12"/>
+        <color indexed="13"/>
         <rFont val="Arial"/>
       </rPr>
       <t>https://wdi-optimised-frontend-starter.vercel.app/news-single.html</t>
@@ -324,6 +324,40 @@
   </si>
   <si>
     <t>Zmienność</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="20"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">21,927
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="20"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>6,037</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="20"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>0.638</t>
+    </r>
+  </si>
+  <si>
+    <t>0.690</t>
   </si>
 </sst>
 </file>
@@ -358,7 +392,7 @@
     <font>
       <u val="single"/>
       <sz val="12"/>
-      <color indexed="12"/>
+      <color indexed="13"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -370,7 +404,7 @@
     <font>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="12"/>
+      <color indexed="13"/>
       <name val="Helvetica Neue"/>
     </font>
     <font>
@@ -383,7 +417,7 @@
       <b val="1"/>
       <u val="single"/>
       <sz val="10"/>
-      <color indexed="12"/>
+      <color indexed="13"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -397,7 +431,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="20">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,7 +440,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="10"/>
+        <fgColor indexed="9"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -418,7 +452,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -486,6 +520,43 @@
         <bgColor auto="1"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="26"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="27"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="28"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="29"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <gradientFill type="linear" degree="270">
+        <stop position="0">
+          <color rgb="ffffecbc"/>
+        </stop>
+        <stop position="0.35">
+          <color rgb="fffff1d0"/>
+        </stop>
+        <stop position="1">
+          <color rgb="fffff9ed"/>
+        </stop>
+      </gradientFill>
+    </fill>
   </fills>
   <borders count="24">
     <border>
@@ -497,11 +568,11 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -510,7 +581,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -518,17 +589,17 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
@@ -545,7 +616,7 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -553,12 +624,12 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -567,28 +638,28 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="14"/>
@@ -599,7 +670,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
         <color indexed="14"/>
@@ -626,7 +697,7 @@
         <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom/>
@@ -727,52 +798,52 @@
         <color indexed="14"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -782,122 +853,119 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="59" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -922,9 +990,6 @@
       <alignment horizontal="right" vertical="bottom" readingOrder="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -933,17 +998,14 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="10" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="11" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="11" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
@@ -952,9 +1014,6 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="12" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="12" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -981,14 +1040,44 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="9" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1007,11 +1096,11 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff5e88b1"/>
       <rgbColor rgb="ffeef3f4"/>
       <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ffbdc0bf"/>
       <rgbColor rgb="ff3f3f3f"/>
@@ -1024,57 +1113,13 @@
       <rgbColor rgb="ffffb1a6"/>
       <rgbColor rgb="ffff8a7a"/>
       <rgbColor rgb="ffed220b"/>
+      <rgbColor rgb="ff50eddb"/>
+      <rgbColor rgb="ffffb1a6"/>
+      <rgbColor rgb="ffffd932"/>
+      <rgbColor rgb="ff8af3e7"/>
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>384340</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>158165</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>824699</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>66624</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp>
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Shape 2"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4397540" y="3258235"/>
-          <a:ext cx="440360" cy="250090"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
-        </a:ln>
-        <a:effectLst/>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2294,127 +2339,127 @@
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
-      <c r="E1" s="23"/>
+      <c r="E1" s="4"/>
     </row>
     <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="24">
+      <c r="A2" t="s" s="23">
         <v>10</v>
       </c>
-      <c r="B2" t="s" s="24">
+      <c r="B2" t="s" s="23">
         <v>11</v>
       </c>
-      <c r="C2" t="s" s="24">
+      <c r="C2" t="s" s="23">
         <v>12</v>
       </c>
-      <c r="D2" t="s" s="24">
+      <c r="D2" t="s" s="23">
         <v>13</v>
       </c>
-      <c r="E2" s="25"/>
+      <c r="E2" s="24"/>
     </row>
     <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="26"/>
-      <c r="B3" s="27"/>
-      <c r="C3" s="28"/>
-      <c r="D3" s="29"/>
-      <c r="E3" s="25"/>
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="24"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" t="s" s="30">
+      <c r="A4" t="s" s="29">
         <v>14</v>
       </c>
-      <c r="B4" t="s" s="31">
+      <c r="B4" t="s" s="30">
         <v>15</v>
       </c>
-      <c r="C4" t="s" s="32">
+      <c r="C4" t="s" s="31">
         <v>16</v>
       </c>
-      <c r="D4" t="s" s="32">
+      <c r="D4" t="s" s="31">
         <v>17</v>
       </c>
-      <c r="E4" s="25"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" t="s" s="30">
+      <c r="A5" t="s" s="29">
         <v>18</v>
       </c>
-      <c r="B5" t="s" s="31">
+      <c r="B5" t="s" s="30">
         <v>19</v>
       </c>
-      <c r="C5" t="s" s="32">
+      <c r="C5" t="s" s="31">
         <v>20</v>
       </c>
-      <c r="D5" t="s" s="32">
+      <c r="D5" t="s" s="31">
         <v>21</v>
       </c>
-      <c r="E5" s="25"/>
+      <c r="E5" s="24"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" t="s" s="30">
+      <c r="A6" t="s" s="29">
         <v>22</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="32">
         <v>0.0002314814814814815</v>
       </c>
-      <c r="C6" t="s" s="32">
+      <c r="C6" t="s" s="31">
         <v>23</v>
       </c>
-      <c r="D6" t="s" s="32">
+      <c r="D6" t="s" s="31">
         <v>17</v>
       </c>
-      <c r="E6" s="25"/>
+      <c r="E6" s="24"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" t="s" s="30">
+      <c r="A7" t="s" s="29">
         <v>24</v>
       </c>
-      <c r="B7" t="s" s="34">
+      <c r="B7" t="s" s="33">
         <v>25</v>
       </c>
-      <c r="C7" t="s" s="32">
+      <c r="C7" t="s" s="31">
         <v>26</v>
       </c>
-      <c r="D7" t="s" s="32">
+      <c r="D7" t="s" s="31">
         <v>27</v>
       </c>
-      <c r="E7" s="25"/>
+      <c r="E7" s="24"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="35"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="37"/>
-      <c r="E8" s="25"/>
+      <c r="A8" s="34"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="35"/>
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="25"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="35"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="24"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="35"/>
-      <c r="B10" s="36"/>
-      <c r="C10" s="37"/>
-      <c r="D10" s="37"/>
-      <c r="E10" s="25"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="35"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="24"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="35"/>
-      <c r="B11" s="36"/>
-      <c r="C11" s="37"/>
-      <c r="D11" s="37"/>
-      <c r="E11" s="38"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/"/>
-    <hyperlink ref="A5" r:id="rId2" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/contact.html"/>
-    <hyperlink ref="A6" r:id="rId3" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/news-listing.html"/>
-    <hyperlink ref="A7" r:id="rId4" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/news-single.html"/>
+    <hyperlink ref="A4" r:id="rId1" location="" tooltip="" display="Czas ładowania strony głównej https://wdi-optimised-frontend-starter.vercel.app/"/>
+    <hyperlink ref="A5" r:id="rId2" location="" tooltip="" display="Czas ładowania strony kontaktowej https://wdi-optimised-frontend-starter.vercel.app/contact.html"/>
+    <hyperlink ref="A6" r:id="rId3" location="" tooltip="" display="Czas ładowania strony z newsami https://wdi-optimised-frontend-starter.vercel.app/news-listing.html"/>
+    <hyperlink ref="A7" r:id="rId4" location="" tooltip="" display="Czas ładowania pojedyńczego newsa https://wdi-optimised-frontend-starter.vercel.app/news-single.html"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -2426,256 +2471,730 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="13.45" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="19.3516" style="39" customWidth="1"/>
-    <col min="2" max="2" width="18" style="39" customWidth="1"/>
-    <col min="3" max="3" width="15.3516" style="39" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="39" customWidth="1"/>
-    <col min="5" max="5" width="15.5" style="39" customWidth="1"/>
-    <col min="6" max="6" width="15.3516" style="39" customWidth="1"/>
-    <col min="7" max="8" width="16.3516" style="39" customWidth="1"/>
-    <col min="9" max="9" width="14.5" style="39" customWidth="1"/>
-    <col min="10" max="16384" width="14.5" style="39" customWidth="1"/>
+    <col min="1" max="1" width="19.3516" style="38" customWidth="1"/>
+    <col min="2" max="2" width="18" style="38" customWidth="1"/>
+    <col min="3" max="3" width="15.3516" style="38" customWidth="1"/>
+    <col min="4" max="4" width="16.3516" style="38" customWidth="1"/>
+    <col min="5" max="5" width="15.5" style="38" customWidth="1"/>
+    <col min="6" max="6" width="15.3516" style="38" customWidth="1"/>
+    <col min="7" max="8" width="16.3516" style="38" customWidth="1"/>
+    <col min="9" max="9" width="14.5" style="38" customWidth="1"/>
+    <col min="10" max="10" width="19.3516" style="66" customWidth="1"/>
+    <col min="11" max="11" width="18" style="66" customWidth="1"/>
+    <col min="12" max="12" width="15.3516" style="66" customWidth="1"/>
+    <col min="13" max="13" width="16.3516" style="66" customWidth="1"/>
+    <col min="14" max="14" width="15.5" style="66" customWidth="1"/>
+    <col min="15" max="15" width="15.3516" style="66" customWidth="1"/>
+    <col min="16" max="17" width="16.3516" style="66" customWidth="1"/>
+    <col min="18" max="18" width="14.5" style="66" customWidth="1"/>
+    <col min="19" max="16384" width="14.5" style="66" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="13.65" customHeight="1">
-      <c r="A1" s="40"/>
-      <c r="B1" t="s" s="41">
+      <c r="A1" s="39"/>
+      <c r="B1" t="s" s="40">
         <v>28</v>
       </c>
-      <c r="C1" t="s" s="41">
+      <c r="C1" t="s" s="40">
         <v>29</v>
       </c>
-      <c r="D1" t="s" s="41">
+      <c r="D1" t="s" s="40">
         <v>30</v>
       </c>
-      <c r="E1" t="s" s="41">
+      <c r="E1" t="s" s="40">
         <v>31</v>
       </c>
-      <c r="F1" t="s" s="41">
+      <c r="F1" t="s" s="40">
         <v>32</v>
       </c>
-      <c r="G1" t="s" s="41">
+      <c r="G1" t="s" s="40">
         <v>33</v>
       </c>
-      <c r="H1" t="s" s="41">
+      <c r="H1" t="s" s="40">
         <v>34</v>
       </c>
-      <c r="I1" t="s" s="42">
+      <c r="I1" t="s" s="41">
         <v>35</v>
       </c>
     </row>
     <row r="2" ht="13.65" customHeight="1">
-      <c r="A2" t="s" s="43">
+      <c r="A2" t="s" s="42">
         <v>36</v>
       </c>
-      <c r="B2" s="44">
+      <c r="B2" s="43">
         <v>0.169</v>
       </c>
-      <c r="C2" s="44">
+      <c r="C2" s="43">
         <v>1.1</v>
       </c>
-      <c r="D2" s="44">
+      <c r="D2" s="43">
         <v>1.048</v>
       </c>
-      <c r="E2" s="45">
+      <c r="E2" s="44">
         <v>11.607</v>
       </c>
-      <c r="F2" t="s" s="47">
+      <c r="F2" t="s" s="45">
         <v>37</v>
       </c>
-      <c r="G2" s="48">
+      <c r="G2" s="46">
         <v>0.091</v>
       </c>
-      <c r="H2" s="49">
+      <c r="H2" s="47">
         <v>0.106</v>
       </c>
-      <c r="I2" s="50">
+      <c r="I2" s="48">
         <v>9</v>
       </c>
     </row>
     <row r="3" ht="13.65" customHeight="1">
-      <c r="A3" t="s" s="43">
+      <c r="A3" t="s" s="42">
         <v>38</v>
       </c>
-      <c r="B3" s="44">
+      <c r="B3" s="43">
         <v>0.242</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="49">
         <v>1.1</v>
       </c>
-      <c r="D3" s="44">
+      <c r="D3" s="43">
         <v>1.037</v>
       </c>
-      <c r="E3" s="52">
+      <c r="E3" s="50">
         <v>5.98</v>
       </c>
-      <c r="F3" t="s" s="54">
+      <c r="F3" t="s" s="51">
         <v>39</v>
       </c>
-      <c r="G3" s="55">
+      <c r="G3" s="52">
         <v>0.005</v>
       </c>
-      <c r="H3" t="s" s="57">
+      <c r="H3" t="s" s="53">
         <v>40</v>
       </c>
-      <c r="I3" s="50">
+      <c r="I3" s="48">
         <v>14</v>
       </c>
     </row>
     <row r="4" ht="13.65" customHeight="1">
-      <c r="A4" t="s" s="43">
+      <c r="A4" t="s" s="42">
         <v>41</v>
       </c>
-      <c r="B4" s="44">
+      <c r="B4" s="43">
         <v>0.248</v>
       </c>
-      <c r="C4" s="44">
+      <c r="C4" s="43">
         <v>1.1</v>
       </c>
-      <c r="D4" s="44">
+      <c r="D4" s="43">
         <v>1.089</v>
       </c>
-      <c r="E4" s="44">
+      <c r="E4" s="43">
         <v>11.2</v>
       </c>
-      <c r="F4" s="58">
+      <c r="F4" s="54">
         <v>10.667</v>
       </c>
-      <c r="G4" s="59">
+      <c r="G4" s="55">
         <v>0.194</v>
       </c>
-      <c r="H4" t="s" s="60">
+      <c r="H4" t="s" s="56">
         <v>42</v>
       </c>
-      <c r="I4" s="50">
+      <c r="I4" s="48">
         <v>6</v>
       </c>
     </row>
     <row r="5" ht="13.65" customHeight="1">
-      <c r="A5" t="s" s="43">
+      <c r="A5" t="s" s="42">
         <v>43</v>
       </c>
-      <c r="B5" s="49">
+      <c r="B5" s="47">
         <v>0.329</v>
       </c>
-      <c r="C5" s="49">
+      <c r="C5" s="47">
         <v>1.1</v>
       </c>
-      <c r="D5" s="49">
+      <c r="D5" s="47">
         <v>1.134</v>
       </c>
-      <c r="E5" s="49">
+      <c r="E5" s="47">
         <v>5.902</v>
       </c>
-      <c r="F5" s="61">
+      <c r="F5" s="57">
         <v>7.458</v>
       </c>
-      <c r="G5" s="59">
+      <c r="G5" s="55">
         <v>0.201</v>
       </c>
-      <c r="H5" s="62">
+      <c r="H5" s="58">
         <v>0.376</v>
       </c>
-      <c r="I5" s="50">
+      <c r="I5" s="48">
         <v>8</v>
       </c>
     </row>
     <row r="6" ht="13.65" customHeight="1">
-      <c r="A6" t="s" s="43">
+      <c r="A6" t="s" s="42">
         <v>44</v>
       </c>
-      <c r="B6" s="63">
+      <c r="B6" s="59">
         <f>STDEV(B2:B5)</f>
         <v>0.0654064217030713</v>
       </c>
-      <c r="C6" s="63">
+      <c r="C6" s="59">
         <f>STDEV(C2:C5)</f>
         <v>0</v>
       </c>
-      <c r="D6" s="63">
+      <c r="D6" s="59">
         <f>STDEV(D2:D5)</f>
         <v>0.0440983748755741</v>
       </c>
-      <c r="E6" s="64">
+      <c r="E6" s="60">
         <f>STDEV(E2:E5)</f>
         <v>3.15831034732181</v>
       </c>
-      <c r="F6" s="65">
+      <c r="F6" s="61">
         <f>STDEV(F2:F5)</f>
         <v>2.26910566082763</v>
       </c>
-      <c r="G6" s="62">
+      <c r="G6" s="58">
         <f>STDEV(G2:G5)</f>
         <v>0.0932250860373251</v>
       </c>
-      <c r="H6" s="62">
+      <c r="H6" s="58">
         <f>STDEV(H2:H5)</f>
         <v>0.190918830920368</v>
       </c>
-      <c r="I6" s="66"/>
+      <c r="I6" s="62"/>
     </row>
     <row r="7" ht="13.65" customHeight="1">
-      <c r="A7" s="67"/>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="68"/>
+      <c r="A7" s="63"/>
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="64"/>
     </row>
     <row r="8" ht="13.65" customHeight="1">
-      <c r="A8" s="68"/>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="G8" s="68"/>
-      <c r="H8" s="68"/>
-      <c r="I8" s="68"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
     </row>
     <row r="9" ht="13.65" customHeight="1">
-      <c r="A9" s="68"/>
-      <c r="B9" s="68"/>
-      <c r="C9" s="68"/>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
     </row>
     <row r="10" ht="13.65" customHeight="1">
-      <c r="A10" s="68"/>
-      <c r="B10" s="68"/>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="68"/>
-      <c r="I10" s="68"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="64"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="64"/>
+      <c r="F10" s="64"/>
+      <c r="G10" s="64"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="64"/>
+    </row>
+    <row r="11" ht="13.45" customHeight="1">
+      <c r="A11" s="2"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" ht="13.45" customHeight="1">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7"/>
+    </row>
+    <row r="13" ht="13.45" customHeight="1">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="7"/>
+    </row>
+    <row r="14" ht="13.45" customHeight="1">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="7"/>
+    </row>
+    <row r="15" ht="13.45" customHeight="1">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="7"/>
+    </row>
+    <row r="16" ht="13.45" customHeight="1">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="7"/>
+    </row>
+    <row r="17" ht="13.45" customHeight="1">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" ht="13.45" customHeight="1">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="7"/>
+    </row>
+    <row r="19" ht="13.45" customHeight="1">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="7"/>
+    </row>
+    <row r="20" ht="13.45" customHeight="1">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="7"/>
+    </row>
+    <row r="21" ht="13.45" customHeight="1">
+      <c r="A21" s="15"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="19"/>
+    </row>
+    <row r="23" ht="13.65" customHeight="1">
+      <c r="J23" s="39"/>
+      <c r="K23" t="s" s="40">
+        <v>28</v>
+      </c>
+      <c r="L23" t="s" s="40">
+        <v>29</v>
+      </c>
+      <c r="M23" t="s" s="40">
+        <v>30</v>
+      </c>
+      <c r="N23" t="s" s="40">
+        <v>31</v>
+      </c>
+      <c r="O23" t="s" s="40">
+        <v>32</v>
+      </c>
+      <c r="P23" t="s" s="40">
+        <v>33</v>
+      </c>
+      <c r="Q23" t="s" s="40">
+        <v>34</v>
+      </c>
+      <c r="R23" t="s" s="41">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" ht="13.65" customHeight="1">
+      <c r="J24" t="s" s="42">
+        <v>36</v>
+      </c>
+      <c r="K24" s="43">
+        <v>0.166</v>
+      </c>
+      <c r="L24" s="67">
+        <v>0.8</v>
+      </c>
+      <c r="M24" s="52">
+        <v>0.782</v>
+      </c>
+      <c r="N24" s="68">
+        <v>17.079</v>
+      </c>
+      <c r="O24" t="s" s="69">
+        <v>45</v>
+      </c>
+      <c r="P24" s="50">
+        <v>0.06900000000000001</v>
+      </c>
+      <c r="Q24" s="57">
+        <v>1.729</v>
+      </c>
+      <c r="R24" s="48">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" ht="13.65" customHeight="1">
+      <c r="J25" t="s" s="42">
+        <v>38</v>
+      </c>
+      <c r="K25" s="43">
+        <v>0.196</v>
+      </c>
+      <c r="L25" s="52">
+        <v>0.6</v>
+      </c>
+      <c r="M25" s="52">
+        <v>0.587</v>
+      </c>
+      <c r="N25" s="50">
+        <v>5.785</v>
+      </c>
+      <c r="O25" t="s" s="70">
+        <v>46</v>
+      </c>
+      <c r="P25" s="49">
+        <v>0.002</v>
+      </c>
+      <c r="Q25" t="s" s="45">
+        <v>47</v>
+      </c>
+      <c r="R25" s="48">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" ht="13.65" customHeight="1">
+      <c r="J26" t="s" s="42">
+        <v>41</v>
+      </c>
+      <c r="K26" s="43">
+        <v>0.171</v>
+      </c>
+      <c r="L26" s="52">
+        <v>0.6</v>
+      </c>
+      <c r="M26" s="52">
+        <v>0.632</v>
+      </c>
+      <c r="N26" s="71">
+        <v>13</v>
+      </c>
+      <c r="O26" s="54">
+        <v>16.5</v>
+      </c>
+      <c r="P26" s="49">
+        <v>0.193</v>
+      </c>
+      <c r="Q26" t="s" s="72">
+        <v>48</v>
+      </c>
+      <c r="R26" s="48">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" ht="13.65" customHeight="1">
+      <c r="J27" t="s" s="42">
+        <v>43</v>
+      </c>
+      <c r="K27" s="47">
+        <v>0.186</v>
+      </c>
+      <c r="L27" s="59">
+        <v>0.6</v>
+      </c>
+      <c r="M27" s="59">
+        <v>0.598</v>
+      </c>
+      <c r="N27" s="47">
+        <v>5.425</v>
+      </c>
+      <c r="O27" s="73">
+        <v>6.981</v>
+      </c>
+      <c r="P27" s="74">
+        <v>0.199</v>
+      </c>
+      <c r="Q27" s="57">
+        <v>0.638</v>
+      </c>
+      <c r="R27" s="48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" ht="13.65" customHeight="1">
+      <c r="J28" t="s" s="42">
+        <v>44</v>
+      </c>
+      <c r="K28" s="59">
+        <f>STDEV(K24:K27)</f>
+        <v>0.0137689263682153</v>
+      </c>
+      <c r="L28" s="59">
+        <f>STDEV(L24:L27)</f>
+        <v>0.1</v>
+      </c>
+      <c r="M28" s="59">
+        <f>STDEV(M24:M27)</f>
+        <v>0.0902233340106649</v>
+      </c>
+      <c r="N28" s="60">
+        <f>STDEV(N24:N27)</f>
+        <v>5.69776888351923</v>
+      </c>
+      <c r="O28" s="61">
+        <f>STDEV(O24:O27)</f>
+        <v>6.73094945011475</v>
+      </c>
+      <c r="P28" s="58">
+        <f>STDEV(P24:P27)</f>
+        <v>0.09664841781771009</v>
+      </c>
+      <c r="Q28" s="58">
+        <f>STDEV(Q24:Q27)</f>
+        <v>0.771453498274523</v>
+      </c>
+      <c r="R28" s="62"/>
+    </row>
+    <row r="29" ht="13.65" customHeight="1">
+      <c r="J29" s="63"/>
+      <c r="K29" s="63"/>
+      <c r="L29" s="63"/>
+      <c r="M29" s="63"/>
+      <c r="N29" s="63"/>
+      <c r="O29" s="63"/>
+      <c r="P29" s="63"/>
+      <c r="Q29" s="63"/>
+      <c r="R29" s="64"/>
+    </row>
+    <row r="30" ht="13.65" customHeight="1">
+      <c r="J30" s="64"/>
+      <c r="K30" s="64"/>
+      <c r="L30" s="64"/>
+      <c r="M30" s="64"/>
+      <c r="N30" s="64"/>
+      <c r="O30" s="64"/>
+      <c r="P30" s="64"/>
+      <c r="Q30" s="64"/>
+      <c r="R30" s="64"/>
+    </row>
+    <row r="31" ht="13.65" customHeight="1">
+      <c r="J31" s="64"/>
+      <c r="K31" s="64"/>
+      <c r="L31" s="64"/>
+      <c r="M31" s="64"/>
+      <c r="N31" s="64"/>
+      <c r="O31" s="64"/>
+      <c r="P31" s="64"/>
+      <c r="Q31" s="64"/>
+      <c r="R31" s="64"/>
+    </row>
+    <row r="32" ht="13.65" customHeight="1">
+      <c r="J32" s="64"/>
+      <c r="K32" s="64"/>
+      <c r="L32" s="64"/>
+      <c r="M32" s="64"/>
+      <c r="N32" s="64"/>
+      <c r="O32" s="64"/>
+      <c r="P32" s="64"/>
+      <c r="Q32" s="64"/>
+      <c r="R32" s="64"/>
+    </row>
+    <row r="33" ht="13.45" customHeight="1">
+      <c r="J33" s="2"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="4"/>
+    </row>
+    <row r="34" ht="13.45" customHeight="1">
+      <c r="J34" s="5"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="6"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="6"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="7"/>
+    </row>
+    <row r="35" ht="13.45" customHeight="1">
+      <c r="J35" s="5"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="7"/>
+    </row>
+    <row r="36" ht="13.45" customHeight="1">
+      <c r="J36" s="5"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="7"/>
+    </row>
+    <row r="37" ht="13.45" customHeight="1">
+      <c r="J37" s="5"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="7"/>
+    </row>
+    <row r="38" ht="13.45" customHeight="1">
+      <c r="J38" s="5"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="7"/>
+    </row>
+    <row r="39" ht="13.45" customHeight="1">
+      <c r="J39" s="5"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="7"/>
+    </row>
+    <row r="40" ht="13.45" customHeight="1">
+      <c r="J40" s="5"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="7"/>
+    </row>
+    <row r="41" ht="13.45" customHeight="1">
+      <c r="J41" s="5"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="7"/>
+    </row>
+    <row r="42" ht="13.45" customHeight="1">
+      <c r="J42" s="5"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="7"/>
+    </row>
+    <row r="43" ht="13.45" customHeight="1">
+      <c r="J43" s="15"/>
+      <c r="K43" s="65"/>
+      <c r="L43" s="65"/>
+      <c r="M43" s="65"/>
+      <c r="N43" s="65"/>
+      <c r="O43" s="65"/>
+      <c r="P43" s="65"/>
+      <c r="Q43" s="65"/>
+      <c r="R43" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/"/>
-    <hyperlink ref="A3" r:id="rId2" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/contact.html"/>
-    <hyperlink ref="A4" r:id="rId3" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/news-listing.html"/>
-    <hyperlink ref="A5" r:id="rId4" location="" tooltip="" display="https://wdi-optimised-frontend-starter.vercel.app/news-single.html"/>
+    <hyperlink ref="A2" r:id="rId1" location="" tooltip="" display="Strona główna https://wdi-optimised-frontend-starter.vercel.app/"/>
+    <hyperlink ref="A3" r:id="rId2" location="" tooltip="" display="Kontakt https://wdi-optimised-frontend-starter.vercel.app/contact.html"/>
+    <hyperlink ref="A4" r:id="rId3" location="" tooltip="" display="News https://wdi-optimised-frontend-starter.vercel.app/news-listing.html"/>
+    <hyperlink ref="A5" r:id="rId4" location="" tooltip="" display="Pojedynczy news https://wdi-optimised-frontend-starter.vercel.app/news-single.html"/>
+    <hyperlink ref="J24" r:id="rId5" location="" tooltip="" display="Strona główna https://wdi-optimised-frontend-starter.vercel.app/"/>
+    <hyperlink ref="J25" r:id="rId6" location="" tooltip="" display="Kontakt https://wdi-optimised-frontend-starter.vercel.app/contact.html"/>
+    <hyperlink ref="J26" r:id="rId7" location="" tooltip="" display="News https://wdi-optimised-frontend-starter.vercel.app/news-listing.html"/>
+    <hyperlink ref="J27" r:id="rId8" location="" tooltip="" display="Pojedynczy news https://wdi-optimised-frontend-starter.vercel.app/news-single.html"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>